<commit_message>
PC1: changed 2  A.xlsx
</commit_message>
<xml_diff>
--- a/A.xlsx
+++ b/A.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torat\Desktop\document\xlsxtest\sample\pc2\xlsx_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torat\Desktop\document\xlsxtest\sample\pc1\xlsx_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9BEC1E-525B-420F-85B2-B45721FD659B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B6818D-1599-4EDD-BABB-89614F415F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11625" yWindow="2363" windowWidth="9945" windowHeight="8775" xr2:uid="{AC4F4AB9-B167-41A4-A1D0-1C01A0D47E10}"/>
   </bookViews>
@@ -31,11 +31,11 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>pc1</t>
+    <t>1-PC</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>pc2</t>
+    <t>2-PC</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -403,7 +403,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>

</xml_diff>

<commit_message>
PC2: A.xlsx 2 chenged
</commit_message>
<xml_diff>
--- a/A.xlsx
+++ b/A.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torat\Desktop\document\xlsxtest\sample\pc2\xlsx_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C9BEC1E-525B-420F-85B2-B45721FD659B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{490E5A4E-F7A4-4F0C-A42E-534AED53E9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11625" yWindow="2363" windowWidth="9945" windowHeight="8775" xr2:uid="{AC4F4AB9-B167-41A4-A1D0-1C01A0D47E10}"/>
   </bookViews>
@@ -25,17 +25,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>aaa</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>pc1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>pc2</t>
+    <t>pc1-pc123</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -400,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE95B70B-971F-45AD-972F-BDB36096A597}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
@@ -418,11 +414,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PC2: A.xlsx order test
</commit_message>
<xml_diff>
--- a/A.xlsx
+++ b/A.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torat\Desktop\document\xlsxtest\sample\pc1\xlsx_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torat\Desktop\document\xlsxtest\sample2\pc2\xlsx_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B6818D-1599-4EDD-BABB-89614F415F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186B3895-8564-4C1C-8678-2FEDBFA08D73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11625" yWindow="2363" windowWidth="9945" windowHeight="8775" xr2:uid="{AC4F4AB9-B167-41A4-A1D0-1C01A0D47E10}"/>
   </bookViews>
@@ -25,17 +25,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>aaa</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>1-PC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2-PC</t>
+    <t>abc</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -403,7 +399,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
@@ -420,7 +416,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.7">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PC1: A.xlsx order test
</commit_message>
<xml_diff>
--- a/A.xlsx
+++ b/A.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torat\Desktop\document\xlsxtest\sample\pc1\xlsx_test\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\torat\Desktop\document\xlsxtest\sample2\pc1\xlsx_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B6818D-1599-4EDD-BABB-89614F415F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB046C86-B08E-4F80-9767-278CA72023F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11625" yWindow="2363" windowWidth="9945" windowHeight="8775" xr2:uid="{AC4F4AB9-B167-41A4-A1D0-1C01A0D47E10}"/>
   </bookViews>
@@ -25,17 +25,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>aaa</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1-PC</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2-PC</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -403,7 +395,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.649999999999999" x14ac:dyDescent="0.7"/>
@@ -414,13 +406,13 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A2" t="s">
-        <v>1</v>
+      <c r="A2">
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.7">
-      <c r="A3" t="s">
-        <v>2</v>
+      <c r="A3">
+        <v>456</v>
       </c>
     </row>
   </sheetData>

</xml_diff>